<commit_message>
formatted tables for journal
</commit_message>
<xml_diff>
--- a/tables/Seasonal Grp Means Table.xlsx
+++ b/tables/Seasonal Grp Means Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewpierson/Desktop/Heloderma Spatial/Heloderma Spatial/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE55C124-0400-DB4F-827C-3493AE8A5BDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99051452-0910-6341-BE84-0D23C8F38CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="920" windowWidth="22840" windowHeight="13600" activeTab="1" xr2:uid="{45E31E4A-E781-9149-8FF7-8A091B9BE969}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="80">
   <si>
     <t>Environment</t>
   </si>
@@ -226,54 +226,6 @@
     <t>df = 67.3,             t = -1.03,               p = 0.72</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">df = 78.9,              t = 5.09,               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p = &lt;0.0001</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">df = 68,                 t = -6.36,                         </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p = &lt;0.0001</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">df = 74,                    t = 6.42,                      </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p = &lt;0.0001</t>
-    </r>
-  </si>
-  <si>
     <t>df = 88.6,             t = 2.54,               p = 0.06</t>
   </si>
   <si>
@@ -289,22 +241,6 @@
     <t>df = 84.9,              t = 1.42,               p = 0.48</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">df = 80.2,             t = 2.66,               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p = 0.04</t>
-    </r>
-  </si>
-  <si>
     <t>df = 31.6,             t = 0.74,               p = 0.46</t>
   </si>
   <si>
@@ -320,22 +256,6 @@
     <t>df = 49,                 t = 0.13,               p = 0.89</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">df = 47.2,             t = -3.65,               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p = 0.0006</t>
-    </r>
-  </si>
-  <si>
     <t>df = 47.1,             t = -1.44,               p = 0.15</t>
   </si>
   <si>
@@ -358,22 +278,6 @@
   </si>
   <si>
     <t>&lt;0.0001</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">df = 69.4,              t = 5.05,               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p = &lt;0.0001</t>
-    </r>
   </si>
   <si>
     <r>
@@ -403,6 +307,36 @@
       <t xml:space="preserve">Post-Hoc comparisons between Owl Head and Stone Canyon across each season. Results are averaged over sex. </t>
     </r>
   </si>
+  <si>
+    <t>df = 47.2,             t = -3.65,               p = 0.0006</t>
+  </si>
+  <si>
+    <t>df = 69.4,              t = 5.05,               p = &lt;0.0001</t>
+  </si>
+  <si>
+    <t>df = 68,                 t = -6.36,                         p = &lt;0.0001</t>
+  </si>
+  <si>
+    <t>df = 78.9,              t = 5.09,               p = &lt;0.0001</t>
+  </si>
+  <si>
+    <t>df = 80.2,             t = 2.66,               p = 0.04</t>
+  </si>
+  <si>
+    <t>df = 74,                    t = 6.42,                      p = &lt;0.0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average = </t>
+  </si>
+  <si>
+    <t>Subsidized</t>
+  </si>
+  <si>
+    <t>Nonsubsidized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nonsubsidized </t>
+  </si>
 </sst>
 </file>
 
@@ -411,7 +345,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -452,6 +386,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -580,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -640,36 +580,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -685,19 +612,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1030,14 +1000,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33" customHeight="1" thickBot="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
@@ -1202,23 +1172,23 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="17" thickBot="1">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
     </row>
     <row r="14" spans="1:16" ht="17" customHeight="1" thickBot="1">
       <c r="A14" s="1" t="s">
@@ -1239,15 +1209,15 @@
       <c r="F14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
     </row>
     <row r="15" spans="1:16" ht="17" customHeight="1">
       <c r="A15" s="3" t="s">
@@ -1672,540 +1642,774 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10161EC2-6DF8-A647-B35C-0C219974520E}">
-  <dimension ref="B3:J31"/>
+  <dimension ref="B3:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:J31"/>
+    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="34" customHeight="1" thickBot="1">
-      <c r="B3" s="43" t="s">
+    <row r="3" spans="2:10" ht="34" customHeight="1">
+      <c r="B3" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+    </row>
+    <row r="4" spans="2:10" ht="34" customHeight="1">
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="46"/>
+      <c r="C7" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="47"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="47"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="48"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="47"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+    </row>
+    <row r="17" spans="2:16" ht="42">
+      <c r="B17" s="47"/>
+      <c r="C17" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="B18" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+    </row>
+    <row r="19" spans="2:16" ht="42">
+      <c r="B19" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" s="47"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+    </row>
+    <row r="21" spans="2:16" ht="42">
+      <c r="B21" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-    </row>
-    <row r="4" spans="2:10" ht="17" thickBot="1">
-      <c r="B4" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="26" t="s">
+    </row>
+    <row r="22" spans="2:16">
+      <c r="B22" s="47"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+    </row>
+    <row r="23" spans="2:16" ht="42">
+      <c r="B23" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="2:10" ht="45">
-      <c r="B11" s="32"/>
-      <c r="C11" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-    </row>
-    <row r="13" spans="2:10" ht="45">
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="18" t="s">
+      <c r="C23" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="20" t="s">
+      <c r="D23" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="17" t="s">
+      <c r="E23" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="45">
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="46" thickBot="1">
-      <c r="B15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="32" customHeight="1" thickBot="1">
-      <c r="B18" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="36" t="s">
+    </row>
+    <row r="26" spans="2:16" ht="32" customHeight="1">
+      <c r="B26" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4">
-        <v>87.7</v>
-      </c>
-      <c r="D20" s="4">
-        <v>-0.3</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="4">
-        <v>88.3</v>
-      </c>
-      <c r="D21" s="4">
-        <v>2.35</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="4">
-        <v>87.2</v>
-      </c>
-      <c r="D22" s="4">
-        <v>4.8099999999999996</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="17" thickBot="1">
-      <c r="B23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="7">
-        <v>89.4</v>
-      </c>
-      <c r="D23" s="7">
-        <v>-0.92</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="17" thickBot="1">
-      <c r="B26" s="41"/>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-    </row>
-    <row r="27" spans="2:10" ht="17" thickBot="1">
-      <c r="B27" s="39" t="s">
+    </row>
+    <row r="27" spans="2:16" ht="32" customHeight="1">
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="M28" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="N28" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="O28" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="P28" s="56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29" s="16"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+    </row>
+    <row r="30" spans="2:16">
+      <c r="B30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="4">
+        <v>87.7</v>
+      </c>
+      <c r="D30" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="K30" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="N30" s="58">
+        <v>87.7</v>
+      </c>
+      <c r="O30" s="58">
+        <v>-0.3</v>
+      </c>
+      <c r="P30" s="58">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16">
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+    </row>
+    <row r="32" spans="2:16">
+      <c r="B32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4">
+        <v>88.3</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2.35</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="K32" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="M32" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="N32" s="58">
+        <v>88.3</v>
+      </c>
+      <c r="O32" s="58">
+        <v>2.35</v>
+      </c>
+      <c r="P32" s="58">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16">
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="2"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+    </row>
+    <row r="34" spans="2:16">
+      <c r="B34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="4">
+        <v>87.2</v>
+      </c>
+      <c r="D34" s="4">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K34" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="M34" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="N34" s="58">
+        <v>87.2</v>
+      </c>
+      <c r="O34" s="58">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="P34" s="58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="2"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="58"/>
+    </row>
+    <row r="36" spans="2:16">
+      <c r="B36" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="29">
+        <v>89.4</v>
+      </c>
+      <c r="D36" s="29">
+        <v>-0.92</v>
+      </c>
+      <c r="E36" s="29">
+        <v>0.35</v>
+      </c>
+      <c r="K36" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="N36" s="46">
+        <v>89.4</v>
+      </c>
+      <c r="O36" s="46">
+        <v>-0.92</v>
+      </c>
+      <c r="P36" s="46">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" ht="17" thickBot="1">
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
+    </row>
+    <row r="40" spans="2:16" ht="17" thickBot="1">
+      <c r="B40" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="38" t="s">
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-    </row>
-    <row r="28" spans="2:10">
-      <c r="B28" s="26" t="s">
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+    </row>
+    <row r="41" spans="2:16">
+      <c r="B41" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C41" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D41" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E41" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F41" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="27" t="s">
+      <c r="G41" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="H41" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="26" t="s">
+      <c r="I41" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="26" t="s">
+      <c r="J41" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="3" t="s">
+    <row r="42" spans="2:16">
+      <c r="B42" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G42" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I42" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="J42" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:10">
-      <c r="B30" s="3" t="s">
+    <row r="43" spans="2:16">
+      <c r="B43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I43" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J43" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="17" thickBot="1">
-      <c r="B31" s="45" t="s">
+    <row r="44" spans="2:16" ht="17" thickBot="1">
+      <c r="B44" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E44" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G44" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H44" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I44" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J44" s="7" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B26:E26"/>
     <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="B39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated ndvi raster code for figures
</commit_message>
<xml_diff>
--- a/tables/Seasonal Grp Means Table.xlsx
+++ b/tables/Seasonal Grp Means Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewpierson/Desktop/Heloderma Spatial/Heloderma Spatial/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E21E09-F0A6-0743-8EBB-EED92DB991C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16814B0F-A70A-AF40-B321-0B0507CEDD0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="920" windowWidth="22840" windowHeight="13600" activeTab="1" xr2:uid="{45E31E4A-E781-9149-8FF7-8A091B9BE969}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="98">
   <si>
     <t>Environment</t>
   </si>
@@ -399,7 +399,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -447,6 +447,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -456,7 +462,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -570,11 +576,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -712,6 +727,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -721,10 +739,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1699,32 +1733,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10161EC2-6DF8-A647-B35C-0C219974520E}">
-  <dimension ref="B3:P42"/>
+  <dimension ref="B3:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30:P38"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.83203125" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="34" customHeight="1">
-      <c r="B3" s="56" t="s">
+    <row r="3" spans="2:21" ht="34" customHeight="1">
+      <c r="B3" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-    </row>
-    <row r="4" spans="2:10" ht="34" customHeight="1">
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+    </row>
+    <row r="4" spans="2:21" ht="34" customHeight="1">
       <c r="B4" s="32"/>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -1735,7 +1773,7 @@
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:21">
       <c r="B5" s="59" t="s">
         <v>68</v>
       </c>
@@ -1749,8 +1787,22 @@
       <c r="H5" s="59"/>
       <c r="I5" s="59"/>
       <c r="J5" s="59"/>
-    </row>
-    <row r="6" spans="2:10">
+      <c r="L5" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+    </row>
+    <row r="6" spans="2:21">
       <c r="B6" s="35" t="s">
         <v>55</v>
       </c>
@@ -1762,8 +1814,20 @@
       <c r="H6" s="36"/>
       <c r="I6" s="36"/>
       <c r="J6" s="36"/>
-    </row>
-    <row r="7" spans="2:10">
+      <c r="L6" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+    </row>
+    <row r="7" spans="2:21">
       <c r="B7" s="37"/>
       <c r="C7" s="37" t="s">
         <v>42</v>
@@ -1789,8 +1853,36 @@
       <c r="J7" s="37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:10">
+      <c r="L7" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="T7" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="U7" s="63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21">
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
@@ -1800,8 +1892,18 @@
       <c r="H8" s="36"/>
       <c r="I8" s="36"/>
       <c r="J8" s="36"/>
-    </row>
-    <row r="9" spans="2:10">
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="62"/>
+      <c r="P8" s="62"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
+    </row>
+    <row r="9" spans="2:21">
       <c r="B9" s="38" t="s">
         <v>43</v>
       </c>
@@ -1829,8 +1931,36 @@
       <c r="J9" s="36" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="10" spans="2:10">
+      <c r="L9" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="O9" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="P9" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="S9" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="T9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="U9" s="62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21">
       <c r="B10" s="38"/>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
@@ -1840,8 +1970,18 @@
       <c r="H10" s="36"/>
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
-    </row>
-    <row r="11" spans="2:10">
+      <c r="L10" s="64"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
+    </row>
+    <row r="11" spans="2:21">
       <c r="B11" s="38" t="s">
         <v>44</v>
       </c>
@@ -1869,8 +2009,36 @@
       <c r="J11" s="36" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="2:10">
+      <c r="L11" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="N11" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="O11" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="S11" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="T11" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="U11" s="62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21">
       <c r="B12" s="38"/>
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
@@ -1880,8 +2048,18 @@
       <c r="H12" s="36"/>
       <c r="I12" s="36"/>
       <c r="J12" s="36"/>
-    </row>
-    <row r="13" spans="2:10">
+      <c r="L12" s="64"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="62"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="62"/>
+    </row>
+    <row r="13" spans="2:21">
       <c r="B13" s="39" t="s">
         <v>73</v>
       </c>
@@ -1909,8 +2087,36 @@
       <c r="J13" s="36" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="14" spans="2:10">
+      <c r="L13" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="N13" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="P13" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="S13" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="T13" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="U13" s="63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21">
       <c r="B14" s="39"/>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
@@ -1921,7 +2127,7 @@
       <c r="I14" s="36"/>
       <c r="J14" s="36"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:21">
       <c r="B15" s="35" t="s">
         <v>54</v>
       </c>
@@ -1934,11 +2140,11 @@
       <c r="I15" s="36"/>
       <c r="J15" s="36"/>
     </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="58" t="s">
+    <row r="16" spans="2:21">
+      <c r="B16" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
@@ -1947,7 +2153,7 @@
       <c r="I16" s="37"/>
       <c r="J16" s="37"/>
     </row>
-    <row r="17" spans="2:16" ht="42">
+    <row r="17" spans="2:17" ht="42">
       <c r="B17" s="38" t="s">
         <v>10</v>
       </c>
@@ -1976,7 +2182,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:17">
       <c r="B18" s="38"/>
       <c r="C18" s="43"/>
       <c r="D18" s="40"/>
@@ -1987,7 +2193,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
     </row>
-    <row r="19" spans="2:16" ht="42">
+    <row r="19" spans="2:17" ht="42">
       <c r="B19" s="38" t="s">
         <v>11</v>
       </c>
@@ -2016,7 +2222,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:17">
       <c r="B20" s="38"/>
       <c r="C20" s="43"/>
       <c r="D20" s="43"/>
@@ -2027,7 +2233,7 @@
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
     </row>
-    <row r="21" spans="2:16" ht="42">
+    <row r="21" spans="2:17" ht="42">
       <c r="B21" s="41" t="s">
         <v>12</v>
       </c>
@@ -2056,21 +2262,21 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:16">
-      <c r="B24" s="55" t="s">
+    <row r="24" spans="2:17">
+      <c r="B24" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-    </row>
-    <row r="25" spans="2:16">
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+    </row>
+    <row r="25" spans="2:17">
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
     </row>
-    <row r="26" spans="2:16">
+    <row r="26" spans="2:17">
       <c r="B26" s="28" t="s">
         <v>9</v>
       </c>
@@ -2084,13 +2290,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:17">
       <c r="B27" s="16"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
     </row>
-    <row r="28" spans="2:16" ht="32" customHeight="1">
+    <row r="28" spans="2:17" ht="32" customHeight="1">
       <c r="B28" s="3" t="s">
         <v>10</v>
       </c>
@@ -2104,13 +2310,13 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="29" spans="2:16" ht="32" customHeight="1">
+    <row r="29" spans="2:17" ht="32" customHeight="1">
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:17">
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -2141,8 +2347,9 @@
       <c r="P30" s="47" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="2:16">
+      <c r="Q30" s="36"/>
+    </row>
+    <row r="31" spans="2:17">
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2153,8 +2360,9 @@
       <c r="N31" s="36"/>
       <c r="O31" s="36"/>
       <c r="P31" s="36"/>
-    </row>
-    <row r="32" spans="2:16">
+      <c r="Q31" s="36"/>
+    </row>
+    <row r="32" spans="2:17">
       <c r="B32" s="3" t="s">
         <v>12</v>
       </c>
@@ -2185,8 +2393,9 @@
       <c r="P32" s="49">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="33" spans="2:16">
+      <c r="Q32" s="49"/>
+    </row>
+    <row r="33" spans="2:17">
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2197,8 +2406,9 @@
       <c r="N33" s="49"/>
       <c r="O33" s="49"/>
       <c r="P33" s="49"/>
-    </row>
-    <row r="34" spans="2:16">
+      <c r="Q33" s="49"/>
+    </row>
+    <row r="34" spans="2:17">
       <c r="B34" s="27" t="s">
         <v>13</v>
       </c>
@@ -2229,16 +2439,18 @@
       <c r="P34" s="49">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="35" spans="2:16">
+      <c r="Q34" s="49"/>
+    </row>
+    <row r="35" spans="2:17">
       <c r="K35" s="48"/>
       <c r="L35" s="38"/>
       <c r="M35" s="38"/>
       <c r="N35" s="49"/>
       <c r="O35" s="49"/>
       <c r="P35" s="49"/>
-    </row>
-    <row r="36" spans="2:16">
+      <c r="Q35" s="49"/>
+    </row>
+    <row r="36" spans="2:17">
       <c r="K36" s="48" t="s">
         <v>12</v>
       </c>
@@ -2257,8 +2469,9 @@
       <c r="P36" s="49" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" ht="17" thickBot="1">
+      <c r="Q36" s="49"/>
+    </row>
+    <row r="37" spans="2:17" ht="17" thickBot="1">
       <c r="B37" s="54"/>
       <c r="C37" s="54"/>
       <c r="D37" s="54"/>
@@ -2274,8 +2487,9 @@
       <c r="N37" s="49"/>
       <c r="O37" s="49"/>
       <c r="P37" s="49"/>
-    </row>
-    <row r="38" spans="2:16" ht="17" thickBot="1">
+      <c r="Q37" s="49"/>
+    </row>
+    <row r="38" spans="2:17" ht="17" thickBot="1">
       <c r="B38" s="52" t="s">
         <v>40</v>
       </c>
@@ -2307,8 +2521,9 @@
       <c r="P38" s="37">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="39" spans="2:16">
+      <c r="Q38" s="36"/>
+    </row>
+    <row r="39" spans="2:17">
       <c r="B39" s="25" t="s">
         <v>1</v>
       </c>
@@ -2337,7 +2552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="2:16">
+    <row r="40" spans="2:17">
       <c r="B40" s="3" t="s">
         <v>43</v>
       </c>
@@ -2366,7 +2581,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="2:16">
+    <row r="41" spans="2:17">
       <c r="B41" s="3" t="s">
         <v>44</v>
       </c>
@@ -2395,7 +2610,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="2:16" ht="17" thickBot="1">
+    <row r="42" spans="2:17" ht="17" thickBot="1">
       <c r="B42" s="30" t="s">
         <v>45</v>
       </c>
@@ -2425,15 +2640,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="R5:U5"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="G5:J5"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="B37:J37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>